<commit_message>
Alteração das perguntas por ids
</commit_message>
<xml_diff>
--- a/arquivos/respostas.xlsx
+++ b/arquivos/respostas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\demet\git\ppca-engenharia-requisitos\arquivos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{832AC5A4-3BEC-43C5-B4AE-DF78A69F175A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83B0E629-3E45-42D2-8393-A472999E3B1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,9 +43,6 @@
     <t>Como você gerenciar os requisitos do seu projeto?</t>
   </si>
   <si>
-    <t>Como você  elicita os requisitos do seu projeto?</t>
-  </si>
-  <si>
     <t>Há alguma metodologia de  Requisitos que você conheça e não aplique? Qual? (Opcional)</t>
   </si>
   <si>
@@ -377,6 +374,9 @@
   </si>
   <si>
     <t>Não há uma técnica específica., Product Backlog Building</t>
+  </si>
+  <si>
+    <t>Como você elicita os requisitos do seu projeto?</t>
   </si>
 </sst>
 </file>
@@ -679,9 +679,9 @@
   </sheetPr>
   <dimension ref="A1:AU29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Y1" sqref="Y1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -689,7 +689,7 @@
     <col min="1" max="47" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:41" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -712,133 +712,133 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Z1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AO1" s="1" t="s">
-        <v>39</v>
-      </c>
     </row>
-    <row r="2" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:41" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>44916.883352696765</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>46</v>
-      </c>
       <c r="K2" s="1">
         <v>5</v>
       </c>
@@ -933,30 +933,30 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:41" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>44916.984636226851</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="G3" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K3" s="1">
         <v>5</v>
@@ -1052,31 +1052,31 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:41" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>44917.324509710648</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>51</v>
-      </c>
       <c r="K4" s="1">
         <v>4</v>
       </c>
@@ -1171,31 +1171,31 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:41" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>44917.335587326394</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="E5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G5" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>55</v>
-      </c>
       <c r="K5" s="1">
         <v>5</v>
       </c>
@@ -1290,34 +1290,34 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:41" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>44917.340569930559</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="H6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J6" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="H6" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="K6" s="1">
         <v>5</v>
       </c>
@@ -1412,33 +1412,33 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:41" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>44917.374576064816</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>63</v>
-      </c>
       <c r="D7" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K7" s="1">
         <v>4</v>
@@ -1534,30 +1534,30 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:41" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>44917.391189745365</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>65</v>
-      </c>
       <c r="E8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F8" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="G8" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K8" s="1">
         <v>1</v>
@@ -1653,31 +1653,31 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:41" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>44917.410803634259</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="G9" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H9" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="H9" s="1" t="s">
-        <v>67</v>
-      </c>
       <c r="K9" s="1">
         <v>2</v>
       </c>
@@ -1772,31 +1772,31 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:41" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>44917.424994351852</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G10" s="1" t="s">
+      <c r="H10" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="H10" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="K10" s="1">
         <v>3</v>
       </c>
@@ -1891,31 +1891,31 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:41" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>44917.43322770833</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G11" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="G11" s="1" t="s">
+      <c r="H11" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H11" s="1" t="s">
-        <v>74</v>
-      </c>
       <c r="K11" s="1">
         <v>4</v>
       </c>
@@ -2010,37 +2010,37 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:41" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>44917.490762175927</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="E12" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F12" s="1" t="s">
+      <c r="G12" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="H12" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="I12" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="I12" s="1" t="s">
+      <c r="J12" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="J12" s="1" t="s">
-        <v>81</v>
-      </c>
       <c r="K12" s="1">
         <v>5</v>
       </c>
@@ -2135,30 +2135,30 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:41" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>44917.512125740745</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="F13" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F13" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="G13" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K13" s="1">
         <v>5</v>
@@ -2254,30 +2254,30 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:41" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>44917.517955810181</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="E14" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="G14" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="E14" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="H14" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K14" s="1">
         <v>3</v>
@@ -2373,31 +2373,31 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:41" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>44917.523297789347</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C15" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F15" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="G15" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H15" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="H15" s="1" t="s">
-        <v>86</v>
-      </c>
       <c r="K15" s="1">
         <v>5</v>
       </c>
@@ -2492,31 +2492,31 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:41" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>44917.664447650459</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D16" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F16" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="E16" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F16" s="1" t="s">
+      <c r="G16" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="G16" s="1" t="s">
+      <c r="H16" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="H16" s="1" t="s">
-        <v>90</v>
-      </c>
       <c r="K16" s="1">
         <v>4</v>
       </c>
@@ -2611,30 +2611,30 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:47" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>44922.619574837961</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K17" s="1">
         <v>5</v>
@@ -2730,34 +2730,34 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:47" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>44922.632833356482</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F18" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="G18" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="G18" s="1" t="s">
+      <c r="H18" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J18" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="H18" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="J18" s="1" t="s">
-        <v>94</v>
-      </c>
       <c r="K18" s="1">
         <v>4</v>
       </c>
@@ -2852,31 +2852,31 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:47" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>44922.688657060186</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C19" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G19" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="D19" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G19" s="1" t="s">
+      <c r="H19" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="H19" s="1" t="s">
-        <v>97</v>
-      </c>
       <c r="K19" s="1">
         <v>5</v>
       </c>
@@ -2971,30 +2971,30 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:47" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>44922.690941851848</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C20" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E20" s="1" t="s">
+      <c r="F20" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="F20" s="1" t="s">
-        <v>100</v>
-      </c>
       <c r="G20" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K20" s="1">
         <v>4</v>
@@ -3090,30 +3090,30 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:47" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>44922.69310856481</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C21" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="E21" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="F21" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F21" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="G21" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K21" s="1">
         <v>5</v>
@@ -3209,30 +3209,30 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:47" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>44922.69708445602</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K22" s="1">
         <v>3</v>
@@ -3328,30 +3328,30 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:47" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>44922.830805729165</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K23" s="1">
         <v>3</v>
@@ -3447,30 +3447,30 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:47" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>44922.906560092597</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C24" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G24" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="D24" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>104</v>
-      </c>
       <c r="H24" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K24" s="1">
         <v>1</v>
@@ -3566,30 +3566,30 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:47" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>44923.369202569447</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E25" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G25" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="F25" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>106</v>
-      </c>
       <c r="H25" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K25" s="1">
         <v>4</v>
@@ -3685,34 +3685,34 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:47" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>44923.584307083336</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G26" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="H26" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="H26" s="1" t="s">
+      <c r="I26" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="I26" s="1" t="s">
-        <v>109</v>
-      </c>
       <c r="K26" s="1">
         <v>3</v>
       </c>
@@ -3807,36 +3807,36 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:47" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:47" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>44923.693954120376</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C27" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="E27" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="F27" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="G27" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="F27" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="G27" s="1" t="s">
+      <c r="H27" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="I27" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="H27" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="I27" s="1" t="s">
-        <v>114</v>
-      </c>
       <c r="J27" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K27" s="1">
         <v>3</v>
@@ -3937,25 +3937,25 @@
         <v>44924.497372685182</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C28" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F28" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="D28" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="E28" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>116</v>
-      </c>
       <c r="G28" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H28" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I28" s="4"/>
       <c r="J28" s="4"/>
@@ -4064,25 +4064,25 @@
         <v>44924.539942129632</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D29" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E29" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="E29" s="4" t="s">
-        <v>43</v>
-      </c>
       <c r="F29" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G29" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="H29" s="5" t="s">
         <v>117</v>
-      </c>
-      <c r="H29" s="5" t="s">
-        <v>118</v>
       </c>
       <c r="I29" s="4"/>
       <c r="J29" s="4"/>

</xml_diff>